<commit_message>
Differential transition rates for vaccine-type and non-vaccine-type HPV based on appropriately weighted highlighted loadUp.m values.
</commit_message>
<xml_diff>
--- a/Config/HPV_parameters.xlsx
+++ b/Config/HPV_parameters.xlsx
@@ -893,21 +893,6 @@
     <t>Vaccine types (16/18).</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Non-Vaccine Types (other high risk). </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> --&gt; Note: #s might be flipped with below, also I think highlighted zeros are wrong</t>
-    </r>
-  </si>
-  <si>
     <t>Natural immunity clearance mulitpliers for HIV-positive.</t>
   </si>
   <si>
@@ -961,8 +946,11 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> --&gt; Note: #s might be flipped with below, also I think highlighted zeros are wrong</t>
+      <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Vaccine Types (other high risk). </t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1088,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1122,6 +1110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1618,7 +1612,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1647,6 +1640,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2358,21 +2352,21 @@
       <c r="U17" s="38"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="115" t="s">
+      <c r="A18" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="115"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="115"/>
-      <c r="F18" s="115" t="s">
-        <v>234</v>
-      </c>
-      <c r="G18" s="115"/>
-      <c r="H18" s="115"/>
-      <c r="I18" s="115"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
+      <c r="F18" s="114" t="s">
+        <v>233</v>
+      </c>
+      <c r="G18" s="114"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="114"/>
       <c r="J18" s="52"/>
-      <c r="K18" s="111"/>
-      <c r="L18" s="111"/>
+      <c r="K18" s="110"/>
+      <c r="L18" s="110"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
       <c r="O18" s="2"/>
@@ -2397,7 +2391,7 @@
         <v>20</v>
       </c>
       <c r="G19" s="79" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H19" s="55" t="s">
         <v>1</v>
@@ -2406,7 +2400,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="52"/>
-      <c r="L19" s="111"/>
+      <c r="L19" s="110"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
       <c r="O19" s="2"/>
@@ -2433,7 +2427,7 @@
       <c r="F20" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="112">
+      <c r="G20" s="111">
         <v>1</v>
       </c>
       <c r="H20" s="56">
@@ -2443,7 +2437,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="52"/>
-      <c r="L20" s="111"/>
+      <c r="L20" s="110"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="2"/>
@@ -2480,7 +2474,7 @@
         <v>4.12</v>
       </c>
       <c r="J21" s="52"/>
-      <c r="K21" s="113"/>
+      <c r="K21" s="112"/>
       <c r="L21" s="52"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2561,13 +2555,13 @@
       <c r="C24" s="53"/>
       <c r="D24" s="53"/>
       <c r="F24" s="43" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
-      <c r="K24" s="114"/>
+      <c r="K24" s="113"/>
       <c r="L24" s="52"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -2578,7 +2572,7 @@
       <c r="C25" s="53"/>
       <c r="D25" s="53"/>
       <c r="F25" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K25" s="61"/>
       <c r="L25" s="2"/>
@@ -2699,12 +2693,12 @@
       <c r="U31" s="38"/>
     </row>
     <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="115" t="s">
+      <c r="A32" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="115"/>
-      <c r="C32" s="115"/>
-      <c r="D32" s="115"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="114"/>
       <c r="K32" s="3"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -2911,12 +2905,12 @@
     </row>
     <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="55"/>
-      <c r="B44" s="116" t="s">
+      <c r="B44" s="115" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="117"/>
-      <c r="D44" s="117"/>
-      <c r="E44" s="118"/>
+      <c r="C44" s="116"/>
+      <c r="D44" s="116"/>
+      <c r="E44" s="117"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
@@ -3281,12 +3275,12 @@
       <c r="W3" s="38"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="114" t="s">
         <v>204</v>
       </c>
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
     </row>
@@ -3448,12 +3442,12 @@
       <c r="W17" s="38"/>
     </row>
     <row r="18" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="115" t="s">
+      <c r="A18" s="114" t="s">
         <v>205</v>
       </c>
-      <c r="B18" s="115"/>
-      <c r="C18" s="115"/>
-      <c r="D18" s="115"/>
+      <c r="B18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
       <c r="E18" s="39"/>
       <c r="F18" s="39"/>
     </row>
@@ -3641,10 +3635,10 @@
       <c r="W31" s="38"/>
     </row>
     <row r="32" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="115" t="s">
+      <c r="A32" s="114" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="115"/>
+      <c r="B32" s="114"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>
@@ -3774,10 +3768,10 @@
       <c r="W40" s="38"/>
     </row>
     <row r="41" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="115" t="s">
+      <c r="A41" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="115"/>
+      <c r="B41" s="114"/>
       <c r="C41" s="39"/>
       <c r="D41" s="39"/>
       <c r="E41" s="39"/>
@@ -4280,11 +4274,11 @@
     </row>
     <row r="72" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="56"/>
-      <c r="B72" s="115" t="s">
+      <c r="B72" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="C72" s="115"/>
-      <c r="D72" s="115"/>
+      <c r="C72" s="114"/>
+      <c r="D72" s="114"/>
       <c r="E72" s="39"/>
       <c r="F72" s="39"/>
       <c r="G72" s="39" t="s">
@@ -9189,8 +9183,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BW113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13122,7 +13116,7 @@
     </row>
     <row r="23" spans="1:75" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="89" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B23" s="86"/>
       <c r="C23" s="86"/>
@@ -14413,7 +14407,7 @@
     </row>
     <row r="43" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="89" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="B43" s="86"/>
       <c r="C43" s="86"/>
@@ -14924,7 +14918,7 @@
       <c r="O50" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P50" s="106">
+      <c r="P50" s="120">
         <f t="array" ref="P50:P65">AH26*AL6:AL21+AH27*BG6:BG21+AH28*CB6:CB21</f>
         <v>0</v>
       </c>
@@ -14952,11 +14946,11 @@
       <c r="X50" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y50" s="106">
+      <c r="Y50" s="120">
         <f t="array" ref="Y50:Y65">AH26*AW6:AW21+AH27*BR6:BR21+AH28*CM6:CM21</f>
         <v>0</v>
       </c>
-      <c r="Z50" s="106">
+      <c r="Z50" s="120">
         <f t="array" ref="Z50:Z65">AH26*AW6:AW21+AH27*BS6:BS21+AH28*CN6:CN21</f>
         <v>0</v>
       </c>
@@ -15011,7 +15005,7 @@
       <c r="O51" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P51" s="106">
+      <c r="P51" s="120">
         <v>0</v>
       </c>
       <c r="Q51" s="27">
@@ -15038,10 +15032,10 @@
       <c r="X51" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y51" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="106">
+      <c r="Y51" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="120">
         <v>0</v>
       </c>
       <c r="AA51" s="27">
@@ -15095,7 +15089,7 @@
       <c r="O52" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P52" s="106">
+      <c r="P52" s="120">
         <v>0</v>
       </c>
       <c r="Q52" s="27">
@@ -15122,10 +15116,10 @@
       <c r="X52" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y52" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z52" s="106">
+      <c r="Y52" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="120">
         <v>0</v>
       </c>
       <c r="AA52" s="27">
@@ -15179,7 +15173,7 @@
       <c r="O53" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P53" s="106">
+      <c r="P53" s="120">
         <v>0</v>
       </c>
       <c r="Q53" s="27">
@@ -15206,10 +15200,10 @@
       <c r="X53" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y53" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z53" s="106">
+      <c r="Y53" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="120">
         <v>0</v>
       </c>
       <c r="AA53" s="27">
@@ -15263,7 +15257,7 @@
       <c r="O54" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P54" s="106">
+      <c r="P54" s="120">
         <v>0</v>
       </c>
       <c r="Q54" s="27">
@@ -15290,10 +15284,10 @@
       <c r="X54" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y54" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="106">
+      <c r="Y54" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="120">
         <v>0</v>
       </c>
       <c r="AA54" s="27">
@@ -15347,7 +15341,7 @@
       <c r="O55" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P55" s="106">
+      <c r="P55" s="120">
         <v>0</v>
       </c>
       <c r="Q55" s="27">
@@ -15374,10 +15368,10 @@
       <c r="X55" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y55" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z55" s="106">
+      <c r="Y55" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="120">
         <v>0</v>
       </c>
       <c r="AA55" s="27">
@@ -15431,7 +15425,7 @@
       <c r="O56" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P56" s="106">
+      <c r="P56" s="120">
         <v>0</v>
       </c>
       <c r="Q56" s="27">
@@ -15458,10 +15452,10 @@
       <c r="X56" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y56" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="106">
+      <c r="Y56" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="120">
         <v>0</v>
       </c>
       <c r="AA56" s="27">
@@ -15515,7 +15509,7 @@
       <c r="O57" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P57" s="106">
+      <c r="P57" s="120">
         <v>0</v>
       </c>
       <c r="Q57" s="27">
@@ -15542,10 +15536,10 @@
       <c r="X57" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y57" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="106">
+      <c r="Y57" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="120">
         <v>0</v>
       </c>
       <c r="AA57" s="27">
@@ -15599,7 +15593,7 @@
       <c r="O58" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P58" s="106">
+      <c r="P58" s="120">
         <v>0</v>
       </c>
       <c r="Q58" s="27">
@@ -15626,10 +15620,10 @@
       <c r="X58" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y58" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z58" s="106">
+      <c r="Y58" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="120">
         <v>0</v>
       </c>
       <c r="AA58" s="27">
@@ -15683,7 +15677,7 @@
       <c r="O59" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P59" s="106">
+      <c r="P59" s="120">
         <v>0</v>
       </c>
       <c r="Q59" s="27">
@@ -15710,10 +15704,10 @@
       <c r="X59" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y59" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="106">
+      <c r="Y59" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="120">
         <v>0</v>
       </c>
       <c r="AA59" s="27">
@@ -15767,7 +15761,7 @@
       <c r="O60" s="27">
         <v>3.9020000000000001E-3</v>
       </c>
-      <c r="P60" s="106">
+      <c r="P60" s="120">
         <v>0</v>
       </c>
       <c r="Q60" s="27">
@@ -15794,10 +15788,10 @@
       <c r="X60" s="27">
         <v>0.17620050000000001</v>
       </c>
-      <c r="Y60" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="106">
+      <c r="Y60" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="120">
         <v>0</v>
       </c>
       <c r="AA60" s="27">
@@ -15824,7 +15818,7 @@
       <c r="O61" s="27">
         <v>3.9020000000000001E-3</v>
       </c>
-      <c r="P61" s="106">
+      <c r="P61" s="120">
         <v>0</v>
       </c>
       <c r="Q61" s="27">
@@ -15851,10 +15845,10 @@
       <c r="X61" s="27">
         <v>0.17620050000000001</v>
       </c>
-      <c r="Y61" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="106">
+      <c r="Y61" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="120">
         <v>0</v>
       </c>
       <c r="AA61" s="27">
@@ -15881,7 +15875,7 @@
       <c r="O62" s="27">
         <v>3.9020000000000001E-3</v>
       </c>
-      <c r="P62" s="106">
+      <c r="P62" s="120">
         <v>0</v>
       </c>
       <c r="Q62" s="27">
@@ -15908,10 +15902,10 @@
       <c r="X62" s="27">
         <v>0.17620050000000001</v>
       </c>
-      <c r="Y62" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="106">
+      <c r="Y62" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="120">
         <v>0</v>
       </c>
       <c r="AA62" s="27">
@@ -15938,7 +15932,7 @@
       <c r="O63" s="27">
         <v>3.9020000000000001E-3</v>
       </c>
-      <c r="P63" s="106">
+      <c r="P63" s="120">
         <v>0</v>
       </c>
       <c r="Q63" s="27">
@@ -15965,10 +15959,10 @@
       <c r="X63" s="27">
         <v>0.17620050000000001</v>
       </c>
-      <c r="Y63" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z63" s="106">
+      <c r="Y63" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z63" s="120">
         <v>0</v>
       </c>
       <c r="AA63" s="27">
@@ -15995,7 +15989,7 @@
       <c r="O64" s="27">
         <v>3.9020000000000005E-3</v>
       </c>
-      <c r="P64" s="106">
+      <c r="P64" s="120">
         <v>0</v>
       </c>
       <c r="Q64" s="27">
@@ -16022,10 +16016,10 @@
       <c r="X64" s="27">
         <v>0.20378033333333334</v>
       </c>
-      <c r="Y64" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z64" s="106">
+      <c r="Y64" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="120">
         <v>0</v>
       </c>
       <c r="AA64" s="27">
@@ -16052,7 +16046,7 @@
       <c r="O65" s="27">
         <v>3.9020000000000005E-3</v>
       </c>
-      <c r="P65" s="106">
+      <c r="P65" s="120">
         <v>0</v>
       </c>
       <c r="Q65" s="27">
@@ -16079,10 +16073,10 @@
       <c r="X65" s="27">
         <v>0.20378033333333334</v>
       </c>
-      <c r="Y65" s="106">
-        <v>0</v>
-      </c>
-      <c r="Z65" s="106">
+      <c r="Y65" s="120">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="120">
         <v>0</v>
       </c>
       <c r="AA65" s="27">
@@ -16111,8 +16105,8 @@
       <c r="J70" s="86"/>
     </row>
     <row r="71" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="109" t="s">
-        <v>230</v>
+      <c r="A71" s="108" t="s">
+        <v>229</v>
       </c>
       <c r="B71" s="88"/>
       <c r="C71" s="88"/>
@@ -16148,20 +16142,20 @@
       <c r="AG71" s="11"/>
     </row>
     <row r="72" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="119" t="s">
+      <c r="A72" s="118" t="s">
         <v>113</v>
       </c>
-      <c r="B72" s="119"/>
+      <c r="B72" s="118"/>
       <c r="C72" s="86"/>
       <c r="D72" s="86"/>
       <c r="I72" s="86"/>
       <c r="J72" s="86"/>
     </row>
     <row r="73" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="107" t="s">
+      <c r="A73" s="106" t="s">
         <v>83</v>
       </c>
-      <c r="B73" s="108">
+      <c r="B73" s="107">
         <f>0.6</f>
         <v>0.6</v>
       </c>
@@ -16171,10 +16165,10 @@
       <c r="H73" s="86"/>
     </row>
     <row r="74" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="107" t="s">
+      <c r="A74" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="B74" s="108">
+      <c r="B74" s="107">
         <f>0.55</f>
         <v>0.55000000000000004</v>
       </c>
@@ -16184,10 +16178,10 @@
       <c r="H74" s="86"/>
     </row>
     <row r="75" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="107" t="s">
+      <c r="A75" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="108">
+      <c r="B75" s="107">
         <f>0.45</f>
         <v>0.45</v>
       </c>
@@ -16197,10 +16191,10 @@
       <c r="H75" s="86"/>
     </row>
     <row r="76" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A76" s="107" t="s">
+      <c r="A76" s="106" t="s">
         <v>114</v>
       </c>
-      <c r="B76" s="108">
+      <c r="B76" s="107">
         <f>0.3</f>
         <v>0.3</v>
       </c>
@@ -16259,7 +16253,7 @@
     </row>
     <row r="82" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="88" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B82" s="88"/>
       <c r="C82" s="88"/>
@@ -16293,7 +16287,7 @@
       <c r="AE82" s="11"/>
     </row>
     <row r="83" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A83" s="110" t="s">
+      <c r="A83" s="109" t="s">
         <v>117</v>
       </c>
       <c r="B83" s="88"/>
@@ -16328,10 +16322,10 @@
       <c r="AE83" s="11"/>
     </row>
     <row r="84" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A84" s="120" t="s">
+      <c r="A84" s="119" t="s">
         <v>115</v>
       </c>
-      <c r="B84" s="120"/>
+      <c r="B84" s="119"/>
       <c r="C84" s="86"/>
       <c r="D84" s="86"/>
       <c r="E84" s="86"/>
@@ -16458,8 +16452,8 @@
       <c r="J93" s="86"/>
     </row>
     <row r="94" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="109" t="s">
-        <v>232</v>
+      <c r="A94" s="108" t="s">
+        <v>231</v>
       </c>
       <c r="B94" s="11"/>
       <c r="C94" s="11"/>
@@ -16493,8 +16487,8 @@
       <c r="AE94" s="11"/>
     </row>
     <row r="95" spans="1:31" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A95" s="110" t="s">
-        <v>233</v>
+      <c r="A95" s="109" t="s">
+        <v>232</v>
       </c>
       <c r="B95" s="11"/>
       <c r="C95" s="11"/>

</xml_diff>

<commit_message>
Update age range descriptions for HPV/Cin/CC transitions to cover all ages in model.
</commit_message>
<xml_diff>
--- a/Config/HPV_parameters.xlsx
+++ b/Config/HPV_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13700" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13700" tabRatio="796" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="HPV" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="265">
   <si>
     <t>Age</t>
   </si>
@@ -1036,9 +1036,6 @@
     </r>
   </si>
   <si>
-    <t>Relative risks by age (ref = 10-25 yo)</t>
-  </si>
-  <si>
     <t xml:space="preserve">We assume that all regression flows out of a compartment flow into the neighboring compartment, and similarly for all progression flows. For example, to calculate progression from CIN1 to CIN2, we add the flows specified for CIN1 --&gt; CIN2 and CIN1 --&gt; CIN3. </t>
   </si>
   <si>
@@ -1067,6 +1064,18 @@
   </si>
   <si>
     <t xml:space="preserve">Non-Vaccine Types (other high risk). </t>
+  </si>
+  <si>
+    <t>`10-24</t>
+  </si>
+  <si>
+    <t>`25-49</t>
+  </si>
+  <si>
+    <t>`50-69</t>
+  </si>
+  <si>
+    <t>Relative risks by age (ref = 10-24 yo)</t>
   </si>
 </sst>
 </file>
@@ -1927,6 +1936,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1945,7 +1955,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3522,18 +3531,18 @@
       <c r="U17" s="38"/>
     </row>
     <row r="18" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="181" t="s">
+      <c r="A18" s="182" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="181"/>
-      <c r="C18" s="181"/>
-      <c r="D18" s="181"/>
-      <c r="F18" s="181" t="s">
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
+      <c r="F18" s="182" t="s">
         <v>233</v>
       </c>
-      <c r="G18" s="181"/>
-      <c r="H18" s="181"/>
-      <c r="I18" s="181"/>
+      <c r="G18" s="182"/>
+      <c r="H18" s="182"/>
+      <c r="I18" s="182"/>
       <c r="J18" s="52"/>
       <c r="K18" s="110"/>
       <c r="L18" s="110"/>
@@ -3863,12 +3872,12 @@
       <c r="U31" s="38"/>
     </row>
     <row r="32" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="181" t="s">
+      <c r="A32" s="182" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="181"/>
-      <c r="C32" s="181"/>
-      <c r="D32" s="181"/>
+      <c r="B32" s="182"/>
+      <c r="C32" s="182"/>
+      <c r="D32" s="182"/>
       <c r="K32" s="3"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
@@ -4075,12 +4084,12 @@
     </row>
     <row r="44" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="55"/>
-      <c r="B44" s="182" t="s">
+      <c r="B44" s="183" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="183"/>
-      <c r="D44" s="183"/>
-      <c r="E44" s="184"/>
+      <c r="C44" s="184"/>
+      <c r="D44" s="184"/>
+      <c r="E44" s="185"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
@@ -4445,12 +4454,12 @@
       <c r="W3" s="38"/>
     </row>
     <row r="4" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="181" t="s">
+      <c r="A4" s="182" t="s">
         <v>204</v>
       </c>
-      <c r="B4" s="181"/>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
+      <c r="B4" s="182"/>
+      <c r="C4" s="182"/>
+      <c r="D4" s="182"/>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
     </row>
@@ -4612,12 +4621,12 @@
       <c r="W17" s="38"/>
     </row>
     <row r="18" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="181" t="s">
+      <c r="A18" s="182" t="s">
         <v>205</v>
       </c>
-      <c r="B18" s="181"/>
-      <c r="C18" s="181"/>
-      <c r="D18" s="181"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="182"/>
+      <c r="D18" s="182"/>
       <c r="E18" s="39"/>
       <c r="F18" s="39"/>
     </row>
@@ -4805,10 +4814,10 @@
       <c r="W31" s="38"/>
     </row>
     <row r="32" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="181" t="s">
+      <c r="A32" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="181"/>
+      <c r="B32" s="182"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>
@@ -4938,10 +4947,10 @@
       <c r="W40" s="38"/>
     </row>
     <row r="41" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="181" t="s">
+      <c r="A41" s="182" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="181"/>
+      <c r="B41" s="182"/>
       <c r="C41" s="39"/>
       <c r="D41" s="39"/>
       <c r="E41" s="39"/>
@@ -5444,11 +5453,11 @@
     </row>
     <row r="72" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="56"/>
-      <c r="B72" s="181" t="s">
+      <c r="B72" s="182" t="s">
         <v>31</v>
       </c>
-      <c r="C72" s="181"/>
-      <c r="D72" s="181"/>
+      <c r="C72" s="182"/>
+      <c r="D72" s="182"/>
       <c r="E72" s="39"/>
       <c r="F72" s="39"/>
       <c r="G72" s="39" t="s">
@@ -10353,8 +10362,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BW113"/>
   <sheetViews>
-    <sheetView topLeftCell="I19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U48" sqref="U48"/>
+    <sheetView topLeftCell="A10" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="M61" sqref="M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14287,7 +14296,7 @@
     </row>
     <row r="23" spans="1:75" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="89" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B23" s="86"/>
       <c r="C23" s="86"/>
@@ -15578,7 +15587,7 @@
     </row>
     <row r="43" spans="1:29" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="89" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B43" s="86"/>
       <c r="C43" s="86"/>
@@ -16089,7 +16098,7 @@
       <c r="O50" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P50" s="187">
+      <c r="P50" s="181">
         <f t="array" ref="P50:P65">AH26*AL6:AL21+AH27*BG6:BG21+AH28*CB6:CB21</f>
         <v>0</v>
       </c>
@@ -16117,11 +16126,11 @@
       <c r="X50" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y50" s="187">
+      <c r="Y50" s="181">
         <f t="array" ref="Y50:Y65">AH26*AW6:AW21+AH27*BR6:BR21+AH28*CM6:CM21</f>
         <v>0</v>
       </c>
-      <c r="Z50" s="187">
+      <c r="Z50" s="181">
         <f t="array" ref="Z50:Z65">AH26*AW6:AW21+AH27*BS6:BS21+AH28*CN6:CN21</f>
         <v>0</v>
       </c>
@@ -16176,7 +16185,7 @@
       <c r="O51" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P51" s="187">
+      <c r="P51" s="181">
         <v>0</v>
       </c>
       <c r="Q51" s="27">
@@ -16203,10 +16212,10 @@
       <c r="X51" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y51" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="187">
+      <c r="Y51" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="181">
         <v>0</v>
       </c>
       <c r="AA51" s="27">
@@ -16260,7 +16269,7 @@
       <c r="O52" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P52" s="187">
+      <c r="P52" s="181">
         <v>0</v>
       </c>
       <c r="Q52" s="27">
@@ -16287,10 +16296,10 @@
       <c r="X52" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y52" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z52" s="187">
+      <c r="Y52" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="181">
         <v>0</v>
       </c>
       <c r="AA52" s="27">
@@ -16344,7 +16353,7 @@
       <c r="O53" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P53" s="187">
+      <c r="P53" s="181">
         <v>0</v>
       </c>
       <c r="Q53" s="27">
@@ -16371,10 +16380,10 @@
       <c r="X53" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y53" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z53" s="187">
+      <c r="Y53" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="181">
         <v>0</v>
       </c>
       <c r="AA53" s="27">
@@ -16428,7 +16437,7 @@
       <c r="O54" s="27">
         <v>3.9218999999999997E-2</v>
       </c>
-      <c r="P54" s="187">
+      <c r="P54" s="181">
         <v>0</v>
       </c>
       <c r="Q54" s="27">
@@ -16455,10 +16464,10 @@
       <c r="X54" s="27">
         <v>7.8895000000000007E-2</v>
       </c>
-      <c r="Y54" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z54" s="187">
+      <c r="Y54" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="181">
         <v>0</v>
       </c>
       <c r="AA54" s="27">
@@ -16512,7 +16521,7 @@
       <c r="O55" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P55" s="187">
+      <c r="P55" s="181">
         <v>0</v>
       </c>
       <c r="Q55" s="27">
@@ -16539,10 +16548,10 @@
       <c r="X55" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y55" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z55" s="187">
+      <c r="Y55" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="181">
         <v>0</v>
       </c>
       <c r="AA55" s="27">
@@ -16596,7 +16605,7 @@
       <c r="O56" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P56" s="187">
+      <c r="P56" s="181">
         <v>0</v>
       </c>
       <c r="Q56" s="27">
@@ -16623,10 +16632,10 @@
       <c r="X56" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y56" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="187">
+      <c r="Y56" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="181">
         <v>0</v>
       </c>
       <c r="AA56" s="27">
@@ -16680,7 +16689,7 @@
       <c r="O57" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P57" s="187">
+      <c r="P57" s="181">
         <v>0</v>
       </c>
       <c r="Q57" s="27">
@@ -16707,10 +16716,10 @@
       <c r="X57" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y57" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="187">
+      <c r="Y57" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="181">
         <v>0</v>
       </c>
       <c r="AA57" s="27">
@@ -16764,7 +16773,7 @@
       <c r="O58" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P58" s="187">
+      <c r="P58" s="181">
         <v>0</v>
       </c>
       <c r="Q58" s="27">
@@ -16791,10 +16800,10 @@
       <c r="X58" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y58" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z58" s="187">
+      <c r="Y58" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="181">
         <v>0</v>
       </c>
       <c r="AA58" s="27">
@@ -16848,7 +16857,7 @@
       <c r="O59" s="27">
         <v>1.1722E-2</v>
       </c>
-      <c r="P59" s="187">
+      <c r="P59" s="181">
         <v>0</v>
       </c>
       <c r="Q59" s="27">
@@ -16875,10 +16884,10 @@
       <c r="X59" s="27">
         <v>0.1312325</v>
       </c>
-      <c r="Y59" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="187">
+      <c r="Y59" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="181">
         <v>0</v>
       </c>
       <c r="AA59" s="27">
@@ -16932,7 +16941,7 @@
       <c r="O60" s="27">
         <v>3.9020000000000001E-3</v>
       </c>
-      <c r="P60" s="187">
+      <c r="P60" s="181">
         <v>0</v>
       </c>
       <c r="Q60" s="27">
@@ -16959,10 +16968,10 @@
       <c r="X60" s="27">
         <v>0.17620050000000001</v>
       </c>
-      <c r="Y60" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="187">
+      <c r="Y60" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="181">
         <v>0</v>
       </c>
       <c r="AA60" s="27">
@@ -16989,7 +16998,7 @@
       <c r="O61" s="27">
         <v>3.9020000000000001E-3</v>
       </c>
-      <c r="P61" s="187">
+      <c r="P61" s="181">
         <v>0</v>
       </c>
       <c r="Q61" s="27">
@@ -17016,10 +17025,10 @@
       <c r="X61" s="27">
         <v>0.17620050000000001</v>
       </c>
-      <c r="Y61" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="187">
+      <c r="Y61" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="181">
         <v>0</v>
       </c>
       <c r="AA61" s="27">
@@ -17046,7 +17055,7 @@
       <c r="O62" s="27">
         <v>3.9020000000000001E-3</v>
       </c>
-      <c r="P62" s="187">
+      <c r="P62" s="181">
         <v>0</v>
       </c>
       <c r="Q62" s="27">
@@ -17073,10 +17082,10 @@
       <c r="X62" s="27">
         <v>0.17620050000000001</v>
       </c>
-      <c r="Y62" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="187">
+      <c r="Y62" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z62" s="181">
         <v>0</v>
       </c>
       <c r="AA62" s="27">
@@ -17103,7 +17112,7 @@
       <c r="O63" s="27">
         <v>3.9020000000000001E-3</v>
       </c>
-      <c r="P63" s="187">
+      <c r="P63" s="181">
         <v>0</v>
       </c>
       <c r="Q63" s="27">
@@ -17130,10 +17139,10 @@
       <c r="X63" s="27">
         <v>0.17620050000000001</v>
       </c>
-      <c r="Y63" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z63" s="187">
+      <c r="Y63" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z63" s="181">
         <v>0</v>
       </c>
       <c r="AA63" s="27">
@@ -17160,7 +17169,7 @@
       <c r="O64" s="27">
         <v>3.9020000000000005E-3</v>
       </c>
-      <c r="P64" s="187">
+      <c r="P64" s="181">
         <v>0</v>
       </c>
       <c r="Q64" s="27">
@@ -17187,10 +17196,10 @@
       <c r="X64" s="27">
         <v>0.20378033333333334</v>
       </c>
-      <c r="Y64" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z64" s="187">
+      <c r="Y64" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="181">
         <v>0</v>
       </c>
       <c r="AA64" s="27">
@@ -17217,7 +17226,7 @@
       <c r="O65" s="27">
         <v>3.9020000000000005E-3</v>
       </c>
-      <c r="P65" s="187">
+      <c r="P65" s="181">
         <v>0</v>
       </c>
       <c r="Q65" s="27">
@@ -17244,10 +17253,10 @@
       <c r="X65" s="27">
         <v>0.20378033333333334</v>
       </c>
-      <c r="Y65" s="187">
-        <v>0</v>
-      </c>
-      <c r="Z65" s="187">
+      <c r="Y65" s="181">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="181">
         <v>0</v>
       </c>
       <c r="AA65" s="27">
@@ -17313,10 +17322,10 @@
       <c r="AG71" s="11"/>
     </row>
     <row r="72" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="185" t="s">
+      <c r="A72" s="186" t="s">
         <v>113</v>
       </c>
-      <c r="B72" s="185"/>
+      <c r="B72" s="186"/>
       <c r="C72" s="86"/>
       <c r="D72" s="86"/>
       <c r="I72" s="86"/>
@@ -17493,10 +17502,10 @@
       <c r="AE83" s="11"/>
     </row>
     <row r="84" spans="1:31" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A84" s="186" t="s">
+      <c r="A84" s="187" t="s">
         <v>115</v>
       </c>
-      <c r="B84" s="186"/>
+      <c r="B84" s="187"/>
       <c r="C84" s="86"/>
       <c r="D84" s="86"/>
       <c r="E84" s="86"/>
@@ -17923,8 +17932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Y29" sqref="Y29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17956,17 +17965,17 @@
     </row>
     <row r="2" spans="1:65" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="175" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:65" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="176" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:65" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="177" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:65" s="37" customFormat="1" x14ac:dyDescent="0.35">
@@ -17981,10 +17990,10 @@
     </row>
     <row r="7" spans="1:65" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B7" s="174" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -19170,10 +19179,10 @@
     </row>
     <row r="25" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B25" s="151" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="C25" s="152">
         <f t="array" ref="C25:C28">(C$18/SUM(C$18:C$20))*(E11:E14 + F11:F14 +G11:G14) + (C19/SUM(C$18:C$20))*(Z11:Z14 + AA11:AA14 + AB11:AB14) + (C$20/SUM(C$18:C$20))*(Z11:Z14+AA11:AA14 +AB11:AB14)*0.95</f>
@@ -19208,7 +19217,7 @@
         <v>0.10196696743063932</v>
       </c>
       <c r="L25" s="151" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="M25" s="154">
         <f t="array" ref="M25:M28">((AU11:AU14 + AV11:AV14 + AW11:AW14) - (Z11:Z14+AA11:AA14 +AB11:AB14)*0.95*(C20/SUM(C20:C21)))/(1-(C20/SUM(C20:C21)))</f>
@@ -19245,7 +19254,7 @@
     </row>
     <row r="26" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B26" s="149" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="C26" s="86">
         <v>0.13448278127147767</v>
@@ -19272,7 +19281,7 @@
         <v>7.8506747135102528E-2</v>
       </c>
       <c r="L26" s="149" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="M26" s="86">
         <v>3.9348954066985652E-2</v>
@@ -19301,7 +19310,7 @@
     </row>
     <row r="27" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B27" s="149" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="C27" s="86">
         <v>9.6298402061855651E-2</v>
@@ -19328,7 +19337,7 @@
         <v>2.746671079613993E-2</v>
       </c>
       <c r="L27" s="149" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="M27" s="86">
         <v>2.7719267942583732E-2</v>
@@ -19413,7 +19422,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B30" s="7" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="77.5" x14ac:dyDescent="0.35">
@@ -19477,7 +19486,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B32" s="178" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="C32" s="179">
         <f t="shared" ref="C32:J34" si="0">C26/C$25</f>
@@ -19513,7 +19522,7 @@
       </c>
       <c r="K32" s="5"/>
       <c r="L32" s="178" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="M32" s="179">
         <f t="shared" ref="M32:T32" si="1">M26/M$25</f>
@@ -19552,7 +19561,7 @@
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B33" s="166" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="C33" s="179">
         <f t="shared" si="0"/>
@@ -19588,7 +19597,7 @@
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="166" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="M33" s="179">
         <f t="shared" ref="M33:T33" si="2">M27/M$25</f>
@@ -19702,7 +19711,7 @@
     </row>
     <row r="36" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B36" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -19756,10 +19765,10 @@
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B38" s="151" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="C38" s="180">
         <f>AVERAGE(C32,M32)</f>
@@ -19796,7 +19805,7 @@
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B39" s="155" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="C39" s="180">
         <f t="shared" ref="C39:C40" si="5">AVERAGE(C33,M33)</f>

</xml_diff>